<commit_message>
Add LaLiga scraper, clean parsing, merge upcoming matches; add beautifulsoup4 and lxml to requirements
</commit_message>
<xml_diff>
--- a/venta.xlsx
+++ b/venta.xlsx
@@ -6146,27 +6146,63 @@
       </c>
     </row>
     <row r="730" ht="15.75" customHeight="1">
-      <c r="B730" s="7"/>
+      <c r="A730" s="3">
+        <v>46020.0</v>
+      </c>
+      <c r="B730" s="6">
+        <v>2561.0</v>
+      </c>
     </row>
     <row r="731" ht="15.75" customHeight="1">
-      <c r="B731" s="7"/>
+      <c r="A731" s="3">
+        <v>46021.0</v>
+      </c>
+      <c r="B731" s="6">
+        <v>2776.93</v>
+      </c>
     </row>
     <row r="732" ht="15.75" customHeight="1">
-      <c r="B732" s="7"/>
+      <c r="A732" s="3">
+        <v>46022.0</v>
+      </c>
+      <c r="B732" s="6">
+        <v>2626.0</v>
+      </c>
     </row>
     <row r="733" ht="15.75" customHeight="1">
-      <c r="B733" s="7"/>
+      <c r="A733" s="3">
+        <v>46023.0</v>
+      </c>
+      <c r="B733" s="6">
+        <v>5206.42</v>
+      </c>
     </row>
     <row r="734" ht="15.75" customHeight="1">
-      <c r="B734" s="7"/>
+      <c r="A734" s="3">
+        <v>46024.0</v>
+      </c>
+      <c r="B734" s="6">
+        <v>2996.03</v>
+      </c>
     </row>
     <row r="735" ht="15.75" customHeight="1">
-      <c r="B735" s="7"/>
+      <c r="A735" s="3">
+        <v>46025.0</v>
+      </c>
+      <c r="B735" s="6">
+        <v>4261.71</v>
+      </c>
     </row>
     <row r="736" ht="15.75" customHeight="1">
-      <c r="B736" s="7"/>
+      <c r="A736" s="3">
+        <v>46026.0</v>
+      </c>
+      <c r="B736" s="6">
+        <v>3392.62</v>
+      </c>
     </row>
     <row r="737" ht="15.75" customHeight="1">
+      <c r="A737" s="3"/>
       <c r="B737" s="7"/>
     </row>
     <row r="738" ht="15.75" customHeight="1">

</xml_diff>